<commit_message>
Defining prediction variable, improving data dictionary
</commit_message>
<xml_diff>
--- a/data/data-dictionary.xlsx
+++ b/data/data-dictionary.xlsx
@@ -1,24 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28016"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mario/Documents/github/costarica-construction/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CienciaDatos\costarica-construction\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14100" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14100" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data-Dictionary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -198,21 +195,6 @@
   </si>
   <si>
     <t>Financiamiento (Marque únicamente el de mayor aporte):</t>
-  </si>
-  <si>
-    <t>7 Lujado, 22 Cerámica, 88 No aplica, 34 Concreto, 33 Porcelanato, 8 Asfalto, 13 Madera, 98 Otros, 99 Ignorado, 9 Mosaico, 11 Terrazo, 5 Planché, 30 Pizarra, 2 Lastre, 1 Tierra, 20 Adoquín, 25 Alfombra, 10 Terrazín, 23 Azulejo, 6 Lavado, 15 Vinil, 12 Losetas, 32 Terrazo madera, 31 Metal, 26 Paladiana, 4 Grava, 21 Pedrín, 18 Linóleo</t>
-  </si>
-  <si>
-    <t>1 Block concreto, 8 Prefabricado, 88 No aplica, 27 Madera-fibrolit, 13 Gypsum, 15 Hierro galvanizado, 11 Fibrolit, 98 Otros, 10 Madera, 5 Fibrocemento, 26 Block-Fibrolit, 99 Ignorado, 25 Block-Madera, 9 Muro seco, 4 Piedra, 6 Zócalo, 2 Concreto armado, 23 Aluminio, 22 Vidrio, 7 Bambú, 24 Repello francés, 21 Policarbonato, 20 Acrílico, 19 Plástico, 18 Decorpanel, 17 Playwood, 16 P.V.C.</t>
-  </si>
-  <si>
-    <t>01 Hierro galvanizado, 88 No aplica, 03 Tejas, 98 Otros, 99 Ignorado, 04 Losa de concreto</t>
-  </si>
-  <si>
-    <t>01 Propio, 99 Ignorado, 02 Alquiler, 03 Vende, 98 Otros</t>
-  </si>
-  <si>
-    <t>99 Ignorado, 06 Bono BANHVI, 09 Propio, 98 Otros, 01 Bancos, 03 Cooperativa, 05 Mutuales, 08 IMAS, 04 INVU, 02 CCSS, 07 INS</t>
   </si>
   <si>
     <t>1 Construcción
@@ -228,6 +210,119 @@
   </si>
   <si>
     <t>POSIBLES RESPUESTAS</t>
+  </si>
+  <si>
+    <t>01 Hierro galvanizado
+88 No aplica
+03 Tejas
+98 Otros
+99 Ignorado
+04 Losa de concreto</t>
+  </si>
+  <si>
+    <t>01 Propio
+99 Ignorado
+02 Alquiler
+03 Vende
+98 Otros</t>
+  </si>
+  <si>
+    <t>99 Ignorado
+06 Bono BANHVI
+09 Propio
+98 Otros
+01 Bancos
+03 Cooperativa
+05 Mutuales
+08 IMAS
+04 INVU
+02 CCSS
+07 INS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 Pizarra
+2 Lastre
+1 Tierra
+20 Adoquín
+25 Alfombra
+10 Terrazín
+23 Azulejo
+6 Lavado
+15 Vinil
+</t>
+  </si>
+  <si>
+    <t>9 Mosaico
+11 Terrazo
+5 Planché
+4 Grava
+21 Pedrín
+12 Losetas
+32 Terrazo madera
+31 Metal
+26 Paladiana</t>
+  </si>
+  <si>
+    <t>7 Lujado
+22 Cerámica
+88 No aplica
+34 Concreto
+33 Porcelanato
+8 Asfalto
+13 Madera
+98 Otros
+99 Ignorado
+18 Linóleo</t>
+  </si>
+  <si>
+    <t>1 Block concreto
+8 Prefabricado
+88 No aplica
+27 Madera-fibrolit
+13 Gypsum
+15 Hierro galvanizado
+11 Fibrolit
+98 Otros
+10 Madera</t>
+  </si>
+  <si>
+    <t>5 Fibrocemento
+26 Block-Fibrolit
+99 Ignorado
+25 Block-Madera
+20 Acrílico
+19 Plástico
+18 Decorpanel
+17 Playwood
+16 P.V.C.</t>
+  </si>
+  <si>
+    <t>9 Muro seco
+4 Piedra
+6 Zócalo
+2 Concreto armado
+23 Aluminio
+22 Vidrio
+7 Bambú
+24 Repello francés
+21 Policarbonato</t>
+  </si>
+  <si>
+    <t>1 San Jose
+2 Alajuela
+3 Heredia
+4 Cartago
+5 Puntarenas
+6 Guanacaste
+7 Limon</t>
+  </si>
+  <si>
+    <t>1 Valle Central
+2 Chorotega
+3 Pacífico Central
+4 Brunca
+5 Huetar Atlantica
+6 Huetar Norte</t>
   </si>
 </sst>
 </file>
@@ -280,18 +375,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -301,6 +402,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -569,21 +673,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="58.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.5" customWidth="1"/>
+    <col min="3" max="3" width="58.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.25" customWidth="1"/>
+    <col min="5" max="5" width="21.625" customWidth="1"/>
+    <col min="6" max="6" width="16.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -593,11 +699,13 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D1" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -607,8 +715,11 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -618,8 +729,11 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -629,8 +743,11 @@
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+      <c r="F4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>23</v>
       </c>
@@ -640,8 +757,11 @@
       <c r="C5" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="80" x14ac:dyDescent="0.2">
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -651,11 +771,13 @@
       <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="D6" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" ht="47.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -665,11 +787,13 @@
       <c r="C7" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -679,8 +803,11 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
+      <c r="F8" s="8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -690,8 +817,11 @@
       <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -701,8 +831,11 @@
       <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
+      <c r="F10" s="8"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -712,8 +845,11 @@
       <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="112" x14ac:dyDescent="0.2">
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+    </row>
+    <row r="12" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -724,10 +860,17 @@
         <v>52</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="128" x14ac:dyDescent="0.2">
+        <v>65</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:7" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -738,10 +881,17 @@
         <v>53</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="43" x14ac:dyDescent="0.2">
+        <v>66</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>29</v>
       </c>
@@ -751,11 +901,13 @@
       <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+      <c r="D14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E14" s="7"/>
+      <c r="F14" s="7"/>
+    </row>
+    <row r="15" spans="1:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -765,11 +917,13 @@
       <c r="C15" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D15" s="4" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="D15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" ht="173.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -779,11 +933,13 @@
       <c r="C16" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -793,8 +949,13 @@
       <c r="C17" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -804,8 +965,11 @@
       <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -815,8 +979,11 @@
       <c r="C19" s="2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -826,8 +993,11 @@
       <c r="C20" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+    </row>
+    <row r="21" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>39</v>
       </c>
@@ -837,8 +1007,34 @@
       <c r="C21" s="2" t="s">
         <v>44</v>
       </c>
+      <c r="D21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="19">
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
+    <mergeCell ref="D21:F21"/>
+    <mergeCell ref="D11:F11"/>
+    <mergeCell ref="D14:F14"/>
+    <mergeCell ref="D15:F15"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="D4:F4"/>
+    <mergeCell ref="D5:F5"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add cat to dataset
</commit_message>
<xml_diff>
--- a/data/data-dictionary.xlsx
+++ b/data/data-dictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="75">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -323,6 +323,19 @@
 4 Brunca
 5 Huetar Atlantica
 6 Huetar Norte</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>Categoria</t>
+  </si>
+  <si>
+    <t>Variable de predicción</t>
+  </si>
+  <si>
+    <t>0 Barato
+1 Caro</t>
   </si>
 </sst>
 </file>
@@ -375,7 +388,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -383,16 +396,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -699,11 +713,11 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -715,9 +729,9 @@
       <c r="C2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -729,9 +743,9 @@
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -743,9 +757,9 @@
       <c r="C4" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -757,9 +771,9 @@
       <c r="C5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -803,9 +817,9 @@
       <c r="C8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -817,9 +831,9 @@
       <c r="C9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -831,9 +845,9 @@
       <c r="C10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -845,9 +859,9 @@
       <c r="C11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:7" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -901,11 +915,11 @@
       <c r="C14" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
     </row>
     <row r="15" spans="1:7" ht="80.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -952,8 +966,8 @@
       <c r="D17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -965,9 +979,9 @@
       <c r="C18" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -979,9 +993,9 @@
       <c r="C19" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -993,9 +1007,9 @@
       <c r="C20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-      <c r="F20" s="8"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="7"/>
     </row>
     <row r="21" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -1010,16 +1024,33 @@
       <c r="D21" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7"/>
+    </row>
+    <row r="22" spans="1:6" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E22" s="7"/>
+      <c r="F22" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
-    <mergeCell ref="D16:F16"/>
-    <mergeCell ref="D17:F17"/>
-    <mergeCell ref="D18:F18"/>
-    <mergeCell ref="D19:F19"/>
-    <mergeCell ref="D20:F20"/>
+  <mergeCells count="20">
+    <mergeCell ref="D22:F22"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="D6:F6"/>
+    <mergeCell ref="D7:F7"/>
+    <mergeCell ref="D8:F8"/>
+    <mergeCell ref="D9:F9"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="D14:F14"/>
@@ -1028,12 +1059,12 @@
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="D4:F4"/>
     <mergeCell ref="D5:F5"/>
-    <mergeCell ref="D1:F1"/>
-    <mergeCell ref="D6:F6"/>
-    <mergeCell ref="D7:F7"/>
-    <mergeCell ref="D8:F8"/>
-    <mergeCell ref="D9:F9"/>
     <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D16:F16"/>
+    <mergeCell ref="D17:F17"/>
+    <mergeCell ref="D18:F18"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>